<commit_message>
🧪 Adjusted reference files to pass direct comparison test
</commit_message>
<xml_diff>
--- a/glotaran/builtin/io/pandas/test/data/reference_parameters.xlsx
+++ b/glotaran/builtin/io/pandas/test/data/reference_parameters.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,27 +446,32 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>expression</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>minimum</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>maximum</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>non-negative</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>vary</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>non-negative</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>expression</t>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>standard-error</t>
         </is>
       </c>
     </row>
@@ -479,15 +484,20 @@
       <c r="B2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="b">
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
         <v>1</v>
       </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -502,15 +512,20 @@
       <c r="B3" t="n">
         <v>2</v>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="b">
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
         <v>1</v>
       </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -525,15 +540,20 @@
       <c r="B4" t="n">
         <v>3</v>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="b">
         <v>0</v>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -548,15 +568,20 @@
       <c r="B5" t="n">
         <v>4</v>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="b">
         <v>0</v>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -571,15 +596,20 @@
       <c r="B6" t="n">
         <v>5</v>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="b">
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
         <v>1</v>
       </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -594,15 +624,20 @@
       <c r="B7" t="n">
         <v>6</v>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="b">
         <v>1</v>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="inlineStr">
         <is>
           <t>None</t>
         </is>
@@ -617,17 +652,22 @@
       <c r="B8" t="n">
         <v>11</v>
       </c>
-      <c r="C8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$verbose_list.all_defaults + $verbose_list.no_defaults</t>
+        </is>
+      </c>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
+      <c r="E8" t="inlineStr"/>
       <c r="F8" t="b">
         <v>0</v>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>$verbose_list.all_defaults + $verbose_list.no_defaults</t>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>None</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
All test are working again.
</commit_message>
<xml_diff>
--- a/glotaran/builtin/io/pandas/test/data/reference_parameters.xlsx
+++ b/glotaran/builtin/io/pandas/test/data/reference_parameters.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -441,37 +441,37 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>expression</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>maximum</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>minimum</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>non_negative</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>standard_error</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>value</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>expression</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>minimum</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>maximum</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>non-negative</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>vary</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>standard-error</t>
         </is>
       </c>
     </row>
@@ -481,26 +481,26 @@
           <t>pure_list.1</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="b">
+      <c r="H2" t="b">
         <v>1</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
       </c>
     </row>
     <row r="3">
@@ -509,26 +509,26 @@
           <t>pure_list.2</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
         <v>2</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="b">
+      <c r="H3" t="b">
         <v>1</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
       </c>
     </row>
     <row r="4">
@@ -537,26 +537,26 @@
           <t>list_with_options.1</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
         <v>3</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
+      <c r="H4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -565,26 +565,26 @@
           <t>list_with_options.2</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
         <v>4</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
+      <c r="H5" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -593,26 +593,26 @@
           <t>verbose_list.all_defaults</t>
         </is>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
         <v>5</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" t="b">
+      <c r="H6" t="b">
         <v>1</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
       </c>
     </row>
     <row r="7">
@@ -621,26 +621,30 @@
           <t>verbose_list.no_defaults</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
         <v>6</v>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
+      <c r="H7" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -649,26 +653,26 @@
           <t>verbose_list.expression_only</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>$verbose_list.all_defaults + $verbose_list.no_defaults</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
         <v>11</v>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>$verbose_list.all_defaults + $verbose_list.no_defaults</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
+      <c r="H8" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>